<commit_message>
Edited Bug Tracker , Test Cases , completed Plan and the SRS
</commit_message>
<xml_diff>
--- a/Bug Tracker_ParaBank.xlsx
+++ b/Bug Tracker_ParaBank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebra\OneDrive\Desktop\para-bank-restful-booker-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E6352409-626F-4033-A8E7-8CE07CD6F1AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E8BE95-A8CF-482E-BA14-DE7D5D6C2DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{786C75D3-26AE-4F8A-9D9A-6FE8CF830892}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
   <si>
     <t>Status</t>
   </si>
@@ -423,6 +423,20 @@
   </si>
   <si>
     <t>High</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to rejester
+3-Search about email field, but it's not found
+4-Back to the priveus page
+5-Go to Contact Us
+6-You have to enter your email</t>
+  </si>
+  <si>
+    <t>The rejestration form doesn't contain an email field</t>
+  </si>
+  <si>
+    <t>The rejestration form containss an email field</t>
   </si>
 </sst>
 </file>
@@ -873,10 +887,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EF2952-DD27-45C9-B247-48119751CCCA}">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" zoomScale="72" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="73" zoomScaleNormal="56" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1472,6 +1486,33 @@
         <v>80</v>
       </c>
     </row>
+    <row r="21" spans="1:9" ht="234" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update TestCases and Bug Tracker Sheets
</commit_message>
<xml_diff>
--- a/Bug Tracker_ParaBank.xlsx
+++ b/Bug Tracker_ParaBank.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gebra\OneDrive\Desktop\para-bank-restful-booker-testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82E8BE95-A8CF-482E-BA14-DE7D5D6C2DED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0796C057-BEBE-41C6-AD01-7747A8197604}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{786C75D3-26AE-4F8A-9D9A-6FE8CF830892}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="164">
   <si>
     <t>Status</t>
   </si>
@@ -438,12 +438,446 @@
   <si>
     <t>The rejestration form containss an email field</t>
   </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid first name</t>
+  </si>
+  <si>
+    <t>FLI02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid last name field
+</t>
+  </si>
+  <si>
+    <t>FLI05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid address field
+</t>
+  </si>
+  <si>
+    <t>FLI08</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid city field</t>
+  </si>
+  <si>
+    <t>FLI11</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid state field</t>
+  </si>
+  <si>
+    <t>FLI14</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to "Forget login info" page
+3-Enter invalid zip code field</t>
+  </si>
+  <si>
+    <t>FLI17</t>
+  </si>
+  <si>
+    <t>System doesn't accept the SSN field</t>
+  </si>
+  <si>
+    <t>System accepts the SSN field</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Enter active username
+3-Enter matching password
+4-Press login button
+5-Enter invalid SSN field
+6-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>FLI20</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid first name field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP02</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid last name field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP05</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid address field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP08</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid city field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP11</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid state field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP14</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid zip code field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP17</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid phone field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP20</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid SSN field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP23</t>
+  </si>
+  <si>
+    <t>System doesn't accept the Username field</t>
+  </si>
+  <si>
+    <t>System accepts the Username field</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid Username field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP26</t>
+  </si>
+  <si>
+    <t>System doesn't accept the Password field</t>
+  </si>
+  <si>
+    <t>System accepts the Password field</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid Password field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP29</t>
+  </si>
+  <si>
+    <t>System doesn't accept the Confirm field</t>
+  </si>
+  <si>
+    <t>System accepts the Confirm field</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester page
+3-Enter invalid Confirm field
+4-Press tab to move to the next field</t>
+  </si>
+  <si>
+    <t>RP32</t>
+  </si>
+  <si>
+    <t>RP35</t>
+  </si>
+  <si>
+    <t>RP36</t>
+  </si>
+  <si>
+    <t>RP37</t>
+  </si>
+  <si>
+    <t>RP38</t>
+  </si>
+  <si>
+    <t>RP39</t>
+  </si>
+  <si>
+    <t>RP40</t>
+  </si>
+  <si>
+    <t>RP41</t>
+  </si>
+  <si>
+    <t>RP42</t>
+  </si>
+  <si>
+    <t>RP43</t>
+  </si>
+  <si>
+    <t>RP44</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter invalid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter invalid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter invalid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter invalid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter invalid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter invalid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter invalid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter invalid Username
+12-Enter valid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter invalid Password
+13-Enter matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>1-Open website via "https://parabank.parasoft.com/parabank/findtrans.htm"
+2-Go to Rejester Page
+3-Enter valid first name
+4-Enter valid last name
+5-Enter valid address
+6-Enter valid city
+7-Enter valid state
+8-Enter valid zip code
+9-Enter valid phone  number
+10-Enter valid SSN
+11-Enter valid Username
+12-Enter valid Password
+13-Enter not matching confirm 
+14-Press Submit</t>
+  </si>
+  <si>
+    <t>System creates a new account</t>
+  </si>
+  <si>
+    <t>System shows an error message indecating that"SSN is invalid"</t>
+  </si>
+  <si>
+    <t>System shows an error message indecating that"Username is invalid"</t>
+  </si>
+  <si>
+    <t>System shows an error message indecating that"Password is invalid"</t>
+  </si>
+  <si>
+    <t>System shows an error message indecating that"Not matching confirm"</t>
+  </si>
+  <si>
+    <t>AP11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open Website via "https://demo.guru99.com/V1"
+2- Go to admin page
+3-Select JDBC or REST (JSON/XML) as the Data Access Mode.
+4-Enter invalid SOAP Endpoint </t>
+  </si>
+  <si>
+    <t>System should not accepts the field</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open Website via "https://demo.guru99.com/V1"
+2- Go to admin page
+3-Select JDBC or REST (JSON/XML) as the Data Access Mode.
+4-Enter invalid REST Endpoint </t>
+  </si>
+  <si>
+    <t>AP14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Open Website via "https://demo.guru99.com/V1"
+2- Go to admin page
+3-Select JDBC or LoanProcessor Service [ WSDL ](JSON/XML) as the Data Access Mode.
+4-Enter invalid LoanProcessor Service [ WSDL ]Endpoint </t>
+  </si>
+  <si>
+    <t>AP17</t>
+  </si>
+  <si>
+    <t>Gehad Ebrahim , Menna Hassan</t>
+  </si>
+  <si>
+    <t>The application should work the same way on all supported devices and browsers</t>
+  </si>
+  <si>
+    <t>The feature does not work correctly on Browser Chrome using Asus Device , but it works fine on other devices/browsers</t>
+  </si>
+  <si>
+    <t>1- Open The Website on Browser Chrome using Asus Device via "https://demo.guru99.com/V1"
+2-Go to Rejester Page
+3-Enter an already registered user’s data
+4-Press submit</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -482,6 +916,12 @@
     <font>
       <sz val="18"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -529,7 +969,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -550,6 +990,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -887,10 +1339,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8EF2952-DD27-45C9-B247-48119751CCCA}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="73" zoomScaleNormal="56" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" topLeftCell="A42" zoomScale="55" zoomScaleNormal="10" workbookViewId="0">
+      <selection activeCell="Q39" sqref="Q39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1513,6 +1965,935 @@
         <v>80</v>
       </c>
     </row>
+    <row r="22" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="140.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="210.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A30" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A31" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H31" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="G32" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A33" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G33" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="187.2" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A38" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="163.80000000000001" x14ac:dyDescent="0.3">
+      <c r="A39" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="G40" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I41" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F42" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G42" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I42" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F43" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G43" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="F44" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I44" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="F45" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="G45" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I45" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I46" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F47" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="G47" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I47" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I48" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" ht="397.8" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="F49" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="G49" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="I49" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="147" x14ac:dyDescent="0.3">
+      <c r="A50" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>154</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G50" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I50" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="147" x14ac:dyDescent="0.3">
+      <c r="A51" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>157</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="F51" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I51" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="168" x14ac:dyDescent="0.3">
+      <c r="A52" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>159</v>
+      </c>
+      <c r="E52" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="G52" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I52" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="147" x14ac:dyDescent="0.3">
+      <c r="A53" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="8"/>
+      <c r="E53" s="11" t="s">
+        <v>163</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>161</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="H53" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="I53" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="G54" s="9"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>